<commit_message>
reflections and losses fixed
</commit_message>
<xml_diff>
--- a/ph_distr_direct_0deg.xlsx
+++ b/ph_distr_direct_0deg.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,79 +443,799 @@
         <v>-487.5</v>
       </c>
       <c r="B2" t="n">
-        <v>0.007991739132933162</v>
+        <v>67.70821423736845</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>-379.1666666666667</v>
+        <v>-477.6515151515151</v>
       </c>
       <c r="B3" t="n">
-        <v>0.007991739132933162</v>
+        <v>68.84594622387698</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>-270.8333333333334</v>
+        <v>-467.8030303030303</v>
       </c>
       <c r="B4" t="n">
-        <v>0.007991739132933162</v>
+        <v>69.94438768081625</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>-162.5</v>
+        <v>-457.9545454545454</v>
       </c>
       <c r="B5" t="n">
-        <v>0.007991739132933162</v>
+        <v>71.00578382513106</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>-54.16666666666669</v>
+        <v>-448.1060606060606</v>
       </c>
       <c r="B6" t="n">
-        <v>0.007991739132933162</v>
+        <v>72.0320328365446</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>54.16666666666663</v>
+        <v>-438.2575757575758</v>
       </c>
       <c r="B7" t="n">
-        <v>0.007991739132933162</v>
+        <v>73.02476122224778</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>162.5</v>
+        <v>-428.4090909090909</v>
       </c>
       <c r="B8" t="n">
-        <v>0.007991739132933162</v>
+        <v>73.98537853740376</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>270.8333333333333</v>
+        <v>-418.5606060606061</v>
       </c>
       <c r="B9" t="n">
-        <v>0.007991739132933162</v>
+        <v>74.91511816236621</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>379.1666666666666</v>
+        <v>-408.7121212121212</v>
       </c>
       <c r="B10" t="n">
-        <v>0.007991739132933162</v>
+        <v>75.81506829496129</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
+        <v>-398.8636363636364</v>
+      </c>
+      <c r="B11" t="n">
+        <v>76.68619591397049</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>-389.0151515151515</v>
+      </c>
+      <c r="B12" t="n">
+        <v>77.52936573473815</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>-379.1666666666667</v>
+      </c>
+      <c r="B13" t="n">
+        <v>78.34535523069553</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>-369.3181818181818</v>
+      </c>
+      <c r="B14" t="n">
+        <v>79.1348668222123</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>-359.469696969697</v>
+      </c>
+      <c r="B15" t="n">
+        <v>79.89853787135502</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>-349.6212121212121</v>
+      </c>
+      <c r="B16" t="n">
+        <v>80.63694885511546</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>-339.7727272727273</v>
+      </c>
+      <c r="B17" t="n">
+        <v>81.35063025367501</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>-329.9242424242424</v>
+      </c>
+      <c r="B18" t="n">
+        <v>82.04006827711518</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>-320.0757575757576</v>
+      </c>
+      <c r="B19" t="n">
+        <v>82.70570975588481</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>-310.2272727272727</v>
+      </c>
+      <c r="B20" t="n">
+        <v>83.34796626957413</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>-300.3787878787879</v>
+      </c>
+      <c r="B21" t="n">
+        <v>83.96721772055008</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>-290.5303030303031</v>
+      </c>
+      <c r="B22" t="n">
+        <v>84.56381539898473</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>-280.6818181818182</v>
+      </c>
+      <c r="B23" t="n">
+        <v>85.13808463115359</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>-270.8333333333334</v>
+      </c>
+      <c r="B24" t="n">
+        <v>85.69032710486272</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>-260.9848484848485</v>
+      </c>
+      <c r="B25" t="n">
+        <v>86.22082289219907</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>-251.1363636363637</v>
+      </c>
+      <c r="B26" t="n">
+        <v>86.72983223681751</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>-241.2878787878788</v>
+      </c>
+      <c r="B27" t="n">
+        <v>87.21759710196585</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>-231.4393939393939</v>
+      </c>
+      <c r="B28" t="n">
+        <v>87.68434257682705</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>-221.5909090909091</v>
+      </c>
+      <c r="B29" t="n">
+        <v>88.13027810721263</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>-211.7424242424242</v>
+      </c>
+      <c r="B30" t="n">
+        <v>88.55559856609688</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>-201.8939393939394</v>
+      </c>
+      <c r="B31" t="n">
+        <v>88.9604852490786</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>-192.0454545454546</v>
+      </c>
+      <c r="B32" t="n">
+        <v>89.34510675050296</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>-182.1969696969697</v>
+      </c>
+      <c r="B33" t="n">
+        <v>89.70961972404129</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>-172.3484848484849</v>
+      </c>
+      <c r="B34" t="n">
+        <v>90.05416959578272</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>-162.5</v>
+      </c>
+      <c r="B35" t="n">
+        <v>90.37889118016065</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>-152.6515151515152</v>
+      </c>
+      <c r="B36" t="n">
+        <v>90.68390925401883</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>-142.8030303030303</v>
+      </c>
+      <c r="B37" t="n">
+        <v>90.96933905421935</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>-132.9545454545455</v>
+      </c>
+      <c r="B38" t="n">
+        <v>91.23528672826478</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>-123.1060606060606</v>
+      </c>
+      <c r="B39" t="n">
+        <v>91.48184974721954</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>-113.2575757575758</v>
+      </c>
+      <c r="B40" t="n">
+        <v>91.70911727495198</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>-103.4090909090909</v>
+      </c>
+      <c r="B41" t="n">
+        <v>91.91717047590436</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>-93.56060606060612</v>
+      </c>
+      <c r="B42" t="n">
+        <v>92.10608282251306</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>-83.71212121212125</v>
+      </c>
+      <c r="B43" t="n">
+        <v>92.2759203489727</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>-73.86363636363637</v>
+      </c>
+      <c r="B44" t="n">
+        <v>92.42674187115961</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>-64.01515151515156</v>
+      </c>
+      <c r="B45" t="n">
+        <v>92.55859919705489</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>-54.16666666666669</v>
+      </c>
+      <c r="B46" t="n">
+        <v>92.67153729237842</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>-44.31818181818187</v>
+      </c>
+      <c r="B47" t="n">
+        <v>92.7655944328593</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>-34.469696969697</v>
+      </c>
+      <c r="B48" t="n">
+        <v>92.84080232990769</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>-24.62121212121218</v>
+      </c>
+      <c r="B49" t="n">
+        <v>92.89718622862574</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>-14.77272727272731</v>
+      </c>
+      <c r="B50" t="n">
+        <v>92.93476499542066</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>-4.924242424242436</v>
+      </c>
+      <c r="B51" t="n">
+        <v>92.95355117372492</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>4.924242424242379</v>
+      </c>
+      <c r="B52" t="n">
+        <v>92.95355102548885</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>14.77272727272725</v>
+      </c>
+      <c r="B53" t="n">
+        <v>92.93476455129678</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>24.62121212121212</v>
+      </c>
+      <c r="B54" t="n">
+        <v>92.89718548981958</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>34.46969696969688</v>
+      </c>
+      <c r="B55" t="n">
+        <v>92.84080129886712</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>44.31818181818176</v>
+      </c>
+      <c r="B56" t="n">
+        <v>92.76559311338093</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>54.16666666666663</v>
+      </c>
+      <c r="B57" t="n">
+        <v>92.6715356883148</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>64.0151515151515</v>
+      </c>
+      <c r="B58" t="n">
+        <v>92.55859731455899</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>73.86363636363637</v>
+      </c>
+      <c r="B59" t="n">
+        <v>92.42673971601388</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>83.71212121212113</v>
+      </c>
+      <c r="B60" t="n">
+        <v>92.27591792828434</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>93.56060606060601</v>
+      </c>
+      <c r="B61" t="n">
+        <v>92.10608014650123</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>103.4090909090909</v>
+      </c>
+      <c r="B62" t="n">
+        <v>91.91716755188421</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>113.2575757575758</v>
+      </c>
+      <c r="B63" t="n">
+        <v>91.70911411367621</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>123.1060606060605</v>
+      </c>
+      <c r="B64" t="n">
+        <v>91.48184636303171</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>132.9545454545454</v>
+      </c>
+      <c r="B65" t="n">
+        <v>91.23528312879665</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>142.8030303030303</v>
+      </c>
+      <c r="B66" t="n">
+        <v>90.96933525919496</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>152.6515151515151</v>
+      </c>
+      <c r="B67" t="n">
+        <v>90.68390527695499</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>162.5</v>
+      </c>
+      <c r="B68" t="n">
+        <v>90.37888703786444</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>172.3484848484848</v>
+      </c>
+      <c r="B69" t="n">
+        <v>90.05416530526742</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>182.1969696969696</v>
+      </c>
+      <c r="B70" t="n">
+        <v>89.70961530296935</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>192.0454545454545</v>
+      </c>
+      <c r="B71" t="n">
+        <v>89.34510222131595</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>201.8939393939394</v>
+      </c>
+      <c r="B72" t="n">
+        <v>88.96048063398379</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>211.7424242424241</v>
+      </c>
+      <c r="B73" t="n">
+        <v>88.55559388817935</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>221.590909090909</v>
+      </c>
+      <c r="B74" t="n">
+        <v>88.13027339478123</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>231.4393939393939</v>
+      </c>
+      <c r="B75" t="n">
+        <v>87.68433785524888</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>241.2878787878788</v>
+      </c>
+      <c r="B76" t="n">
+        <v>87.21759239688026</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>251.1363636363636</v>
+      </c>
+      <c r="B77" t="n">
+        <v>86.72982757996306</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>260.9848484848484</v>
+      </c>
+      <c r="B78" t="n">
+        <v>86.22081832065794</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>270.8333333333333</v>
+      </c>
+      <c r="B79" t="n">
+        <v>85.69032264718678</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>280.6818181818181</v>
+      </c>
+      <c r="B80" t="n">
+        <v>85.13808032879319</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>290.530303030303</v>
+      </c>
+      <c r="B81" t="n">
+        <v>84.56381129489313</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>300.3787878787878</v>
+      </c>
+      <c r="B82" t="n">
+        <v>83.96721385297144</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>310.2272727272726</v>
+      </c>
+      <c r="B83" t="n">
+        <v>83.34796268719742</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>320.0757575757575</v>
+      </c>
+      <c r="B84" t="n">
+        <v>82.70570649882723</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>329.9242424242424</v>
+      </c>
+      <c r="B85" t="n">
+        <v>82.04006540236168</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>339.7727272727273</v>
+      </c>
+      <c r="B86" t="n">
+        <v>81.35062781325325</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>349.621212121212</v>
+      </c>
+      <c r="B87" t="n">
+        <v>80.63694691497511</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>359.4696969696969</v>
+      </c>
+      <c r="B88" t="n">
+        <v>79.89853649075707</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>369.3181818181818</v>
+      </c>
+      <c r="B89" t="n">
+        <v>79.13486607577212</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>379.1666666666666</v>
+      </c>
+      <c r="B90" t="n">
+        <v>78.34535518322264</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>389.0151515151515</v>
+      </c>
+      <c r="B91" t="n">
+        <v>77.52936647112182</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>398.8636363636363</v>
+      </c>
+      <c r="B92" t="n">
+        <v>76.6861975211537</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>408.7121212121211</v>
+      </c>
+      <c r="B93" t="n">
+        <v>75.81507086409798</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>418.560606060606</v>
+      </c>
+      <c r="B94" t="n">
+        <v>74.91512180838711</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>428.4090909090909</v>
+      </c>
+      <c r="B95" t="n">
+        <v>73.98538336886341</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>438.2575757575756</v>
+      </c>
+      <c r="B96" t="n">
+        <v>73.02476737314021</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>448.1060606060605</v>
+      </c>
+      <c r="B97" t="n">
+        <v>72.03204044582816</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>457.9545454545454</v>
+      </c>
+      <c r="B98" t="n">
+        <v>71.00579305824496</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>467.8030303030303</v>
+      </c>
+      <c r="B99" t="n">
+        <v>69.94439871639264</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>477.6515151515151</v>
+      </c>
+      <c r="B100" t="n">
+        <v>68.84595929066282</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
         <v>487.5</v>
       </c>
-      <c r="B11" t="n">
-        <v>0.007991739132933162</v>
+      <c r="B101" t="n">
+        <v>67.70822957824407</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
transfer from my pc to uts
</commit_message>
<xml_diff>
--- a/ph_distr_direct_0deg.xlsx
+++ b/ph_distr_direct_0deg.xlsx
@@ -382,7 +382,7 @@
         <v>-0.4875</v>
       </c>
       <c r="B2">
-        <v>-375.9946102205495</v>
+        <v>-247.4245882215916</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -390,7 +390,7 @@
         <v>-0.4776515151515152</v>
       </c>
       <c r="B3">
-        <v>-375.9946099522178</v>
+        <v>-247.42458795326</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -398,7 +398,7 @@
         <v>-0.4678030303030303</v>
       </c>
       <c r="B4">
-        <v>-375.9946096838861</v>
+        <v>-247.4245876849283</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -406,7 +406,7 @@
         <v>-0.4579545454545455</v>
       </c>
       <c r="B5">
-        <v>-375.9946094155545</v>
+        <v>-247.4245874165966</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -414,7 +414,7 @@
         <v>-0.4481060606060606</v>
       </c>
       <c r="B6">
-        <v>-375.9946091472227</v>
+        <v>-247.4245871482649</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -422,7 +422,7 @@
         <v>-0.4382575757575758</v>
       </c>
       <c r="B7">
-        <v>-375.9946088788911</v>
+        <v>-247.4245868799333</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -430,7 +430,7 @@
         <v>-0.428409090909091</v>
       </c>
       <c r="B8">
-        <v>-375.9946086105593</v>
+        <v>-247.4245866116016</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -438,7 +438,7 @@
         <v>-0.4185606060606061</v>
       </c>
       <c r="B9">
-        <v>-375.9946083422277</v>
+        <v>-247.4245863432699</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -446,7 +446,7 @@
         <v>-0.4087121212121212</v>
       </c>
       <c r="B10">
-        <v>-375.9946080738961</v>
+        <v>-247.4245860749382</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -454,7 +454,7 @@
         <v>-0.3988636363636364</v>
       </c>
       <c r="B11">
-        <v>-375.9946078055643</v>
+        <v>-247.4245858066066</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -462,7 +462,7 @@
         <v>-0.3890151515151515</v>
       </c>
       <c r="B12">
-        <v>-375.9946075372327</v>
+        <v>-247.4245855382749</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -470,7 +470,7 @@
         <v>-0.3791666666666667</v>
       </c>
       <c r="B13">
-        <v>-375.9946072689011</v>
+        <v>-247.4245852699432</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -478,7 +478,7 @@
         <v>-0.3693181818181819</v>
       </c>
       <c r="B14">
-        <v>-375.9946070005694</v>
+        <v>-247.4245850016115</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -486,7 +486,7 @@
         <v>-0.359469696969697</v>
       </c>
       <c r="B15">
-        <v>-375.9946067322377</v>
+        <v>-247.4245847332799</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -494,7 +494,7 @@
         <v>-0.3496212121212122</v>
       </c>
       <c r="B16">
-        <v>-375.9946064639061</v>
+        <v>-247.4245844649482</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -502,7 +502,7 @@
         <v>-0.3397727272727273</v>
       </c>
       <c r="B17">
-        <v>-375.9946061955743</v>
+        <v>-247.4245841966165</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -510,7 +510,7 @@
         <v>-0.3299242424242425</v>
       </c>
       <c r="B18">
-        <v>-375.9946059272427</v>
+        <v>-247.4245839282849</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -518,7 +518,7 @@
         <v>-0.3200757575757576</v>
       </c>
       <c r="B19">
-        <v>-375.994605658911</v>
+        <v>-247.4245836599532</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -526,7 +526,7 @@
         <v>-0.3102272727272727</v>
       </c>
       <c r="B20">
-        <v>-375.9946053905793</v>
+        <v>-247.4245833916215</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -534,7 +534,7 @@
         <v>-0.3003787878787879</v>
       </c>
       <c r="B21">
-        <v>-375.9946051222477</v>
+        <v>-247.4245831232898</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -542,7 +542,7 @@
         <v>-0.290530303030303</v>
       </c>
       <c r="B22">
-        <v>-375.9946048539159</v>
+        <v>-247.4245828549582</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -550,7 +550,7 @@
         <v>-0.2806818181818182</v>
       </c>
       <c r="B23">
-        <v>-375.9946045855843</v>
+        <v>-247.4245825866265</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -558,7 +558,7 @@
         <v>-0.2708333333333334</v>
       </c>
       <c r="B24">
-        <v>-375.9946043172527</v>
+        <v>-247.4245823182948</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -566,7 +566,7 @@
         <v>-0.2609848484848485</v>
       </c>
       <c r="B25">
-        <v>-375.994604048921</v>
+        <v>-247.4245820499631</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -574,7 +574,7 @@
         <v>-0.2511363636363637</v>
       </c>
       <c r="B26">
-        <v>-375.9946037805893</v>
+        <v>-247.4245817816315</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -582,7 +582,7 @@
         <v>-0.2412878787878788</v>
       </c>
       <c r="B27">
-        <v>-375.9946035122576</v>
+        <v>-247.4245815132998</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -590,7 +590,7 @@
         <v>-0.2314393939393939</v>
       </c>
       <c r="B28">
-        <v>-375.994603243926</v>
+        <v>-247.4245812449682</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -598,7 +598,7 @@
         <v>-0.2215909090909091</v>
       </c>
       <c r="B29">
-        <v>-375.9946029755943</v>
+        <v>-247.4245809766365</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -606,7 +606,7 @@
         <v>-0.2117424242424243</v>
       </c>
       <c r="B30">
-        <v>-375.9946027072626</v>
+        <v>-247.4245807083048</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -614,7 +614,7 @@
         <v>-0.2018939393939394</v>
       </c>
       <c r="B31">
-        <v>-375.9946024389309</v>
+        <v>-247.4245804399731</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -622,7 +622,7 @@
         <v>-0.1920454545454546</v>
       </c>
       <c r="B32">
-        <v>-375.9946021705993</v>
+        <v>-247.4245801716414</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -630,7 +630,7 @@
         <v>-0.1821969696969697</v>
       </c>
       <c r="B33">
-        <v>-375.9946019022675</v>
+        <v>-247.4245799033098</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -638,7 +638,7 @@
         <v>-0.1723484848484849</v>
       </c>
       <c r="B34">
-        <v>-375.9946016339359</v>
+        <v>-247.4245796349781</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -646,7 +646,7 @@
         <v>-0.1625</v>
       </c>
       <c r="B35">
-        <v>-375.9946013656042</v>
+        <v>-247.4245793666464</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -654,7 +654,7 @@
         <v>-0.1526515151515151</v>
       </c>
       <c r="B36">
-        <v>-375.9946010972726</v>
+        <v>-247.4245790983147</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -662,7 +662,7 @@
         <v>-0.1428030303030303</v>
       </c>
       <c r="B37">
-        <v>-375.9946008289409</v>
+        <v>-247.4245788299831</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -670,7 +670,7 @@
         <v>-0.1329545454545454</v>
       </c>
       <c r="B38">
-        <v>-375.9946005606092</v>
+        <v>-247.4245785616514</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -678,7 +678,7 @@
         <v>-0.1231060606060606</v>
       </c>
       <c r="B39">
-        <v>-375.9946002922776</v>
+        <v>-247.4245782933197</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -686,7 +686,7 @@
         <v>-0.1132575757575758</v>
       </c>
       <c r="B40">
-        <v>-375.9946000239458</v>
+        <v>-247.4245780249881</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -694,7 +694,7 @@
         <v>-0.1034090909090909</v>
       </c>
       <c r="B41">
-        <v>-375.9945997556142</v>
+        <v>-247.4245777566564</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -702,7 +702,7 @@
         <v>-0.09356060606060607</v>
       </c>
       <c r="B42">
-        <v>-375.9945994872825</v>
+        <v>-247.4245774883247</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -710,7 +710,7 @@
         <v>-0.08371212121212124</v>
       </c>
       <c r="B43">
-        <v>-375.9945992189508</v>
+        <v>-247.4245772199931</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -718,7 +718,7 @@
         <v>-0.07386363636363635</v>
       </c>
       <c r="B44">
-        <v>-375.9945989506192</v>
+        <v>-247.4245769516614</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -726,7 +726,7 @@
         <v>-0.06401515151515152</v>
       </c>
       <c r="B45">
-        <v>-375.9945986822875</v>
+        <v>-247.4245766833297</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -734,7 +734,7 @@
         <v>-0.0541666666666667</v>
       </c>
       <c r="B46">
-        <v>-375.9945984139558</v>
+        <v>-247.424576414998</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -742,7 +742,7 @@
         <v>-0.04431818181818181</v>
       </c>
       <c r="B47">
-        <v>-375.9945981456242</v>
+        <v>-247.4245761466663</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -750,7 +750,7 @@
         <v>-0.03446969696969698</v>
       </c>
       <c r="B48">
-        <v>-375.9945978772924</v>
+        <v>-247.4245758783347</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -758,7 +758,7 @@
         <v>-0.0246212121212121</v>
       </c>
       <c r="B49">
-        <v>-375.9945976089608</v>
+        <v>-247.424575610003</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -766,7 +766,7 @@
         <v>-0.01477272727272727</v>
       </c>
       <c r="B50">
-        <v>-375.9945973406292</v>
+        <v>-247.4245753416713</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -774,7 +774,7 @@
         <v>-0.004924242424242442</v>
       </c>
       <c r="B51">
-        <v>-375.9945970722974</v>
+        <v>-247.4245750733397</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -782,7 +782,7 @@
         <v>0.004924242424242442</v>
       </c>
       <c r="B52">
-        <v>-375.9945968039658</v>
+        <v>-247.424574805008</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -790,7 +790,7 @@
         <v>0.01477272727272727</v>
       </c>
       <c r="B53">
-        <v>-375.9945965356341</v>
+        <v>-247.4245745366763</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -798,7 +798,7 @@
         <v>0.02462121212121215</v>
       </c>
       <c r="B54">
-        <v>-375.9945962673024</v>
+        <v>-247.4245742683447</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -806,7 +806,7 @@
         <v>0.03446969696969693</v>
       </c>
       <c r="B55">
-        <v>-375.9945959989708</v>
+        <v>-247.424574000013</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -814,7 +814,7 @@
         <v>0.04431818181818181</v>
       </c>
       <c r="B56">
-        <v>-375.994595730639</v>
+        <v>-247.4245737316813</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -822,7 +822,7 @@
         <v>0.0541666666666667</v>
       </c>
       <c r="B57">
-        <v>-375.9945954623074</v>
+        <v>-247.4245734633496</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -830,7 +830,7 @@
         <v>0.06401515151515147</v>
       </c>
       <c r="B58">
-        <v>-375.9945951939758</v>
+        <v>-247.4245731950179</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -838,7 +838,7 @@
         <v>0.07386363636363635</v>
       </c>
       <c r="B59">
-        <v>-375.994594925644</v>
+        <v>-247.4245729266863</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -846,7 +846,7 @@
         <v>0.08371212121212124</v>
       </c>
       <c r="B60">
-        <v>-375.9945946573124</v>
+        <v>-247.4245726583546</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -854,7 +854,7 @@
         <v>0.09356060606060612</v>
       </c>
       <c r="B61">
-        <v>-375.9945943889808</v>
+        <v>-247.4245723900229</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -862,7 +862,7 @@
         <v>0.1034090909090909</v>
       </c>
       <c r="B62">
-        <v>-375.994594120649</v>
+        <v>-247.4245721216913</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -870,7 +870,7 @@
         <v>0.1132575757575758</v>
       </c>
       <c r="B63">
-        <v>-375.9945938523174</v>
+        <v>-247.4245718533596</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -878,7 +878,7 @@
         <v>0.1231060606060607</v>
       </c>
       <c r="B64">
-        <v>-375.9945935839856</v>
+        <v>-247.4245715850279</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -886,7 +886,7 @@
         <v>0.1329545454545454</v>
       </c>
       <c r="B65">
-        <v>-375.994593315654</v>
+        <v>-247.4245713166962</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -894,7 +894,7 @@
         <v>0.1428030303030303</v>
       </c>
       <c r="B66">
-        <v>-375.9945930473224</v>
+        <v>-247.4245710483646</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -902,7 +902,7 @@
         <v>0.1526515151515152</v>
       </c>
       <c r="B67">
-        <v>-375.9945927789906</v>
+        <v>-247.4245707800329</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -910,7 +910,7 @@
         <v>0.1625</v>
       </c>
       <c r="B68">
-        <v>-375.994592510659</v>
+        <v>-247.4245705117012</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -918,7 +918,7 @@
         <v>0.1723484848484849</v>
       </c>
       <c r="B69">
-        <v>-375.9945922423274</v>
+        <v>-247.4245702433695</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -926,7 +926,7 @@
         <v>0.1821969696969697</v>
       </c>
       <c r="B70">
-        <v>-375.9945919739957</v>
+        <v>-247.4245699750379</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -934,7 +934,7 @@
         <v>0.1920454545454545</v>
       </c>
       <c r="B71">
-        <v>-375.994591705664</v>
+        <v>-247.4245697067062</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -942,7 +942,7 @@
         <v>0.2018939393939394</v>
       </c>
       <c r="B72">
-        <v>-375.9945914373324</v>
+        <v>-247.4245694383745</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -950,7 +950,7 @@
         <v>0.2117424242424243</v>
       </c>
       <c r="B73">
-        <v>-375.9945911690006</v>
+        <v>-247.4245691700428</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -958,7 +958,7 @@
         <v>0.2215909090909092</v>
       </c>
       <c r="B74">
-        <v>-375.994590900669</v>
+        <v>-247.4245689017112</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -966,7 +966,7 @@
         <v>0.2314393939393939</v>
       </c>
       <c r="B75">
-        <v>-375.9945906323372</v>
+        <v>-247.4245686333795</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -974,7 +974,7 @@
         <v>0.2412878787878788</v>
       </c>
       <c r="B76">
-        <v>-375.9945903640056</v>
+        <v>-247.4245683650478</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -982,7 +982,7 @@
         <v>0.2511363636363637</v>
       </c>
       <c r="B77">
-        <v>-375.994590095674</v>
+        <v>-247.4245680967161</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -990,7 +990,7 @@
         <v>0.2609848484848485</v>
       </c>
       <c r="B78">
-        <v>-375.9945898273422</v>
+        <v>-247.4245678283845</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -998,7 +998,7 @@
         <v>0.2708333333333334</v>
       </c>
       <c r="B79">
-        <v>-375.9945895590106</v>
+        <v>-247.4245675600528</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1006,7 +1006,7 @@
         <v>0.2806818181818183</v>
       </c>
       <c r="B80">
-        <v>-375.994589290679</v>
+        <v>-247.4245672917211</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1014,7 +1014,7 @@
         <v>0.290530303030303</v>
       </c>
       <c r="B81">
-        <v>-375.9945890223473</v>
+        <v>-247.4245670233894</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1022,7 +1022,7 @@
         <v>0.3003787878787879</v>
       </c>
       <c r="B82">
-        <v>-375.9945887540156</v>
+        <v>-247.4245667550578</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1030,7 +1030,7 @@
         <v>0.3102272727272728</v>
       </c>
       <c r="B83">
-        <v>-375.9945884856839</v>
+        <v>-247.4245664867261</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1038,7 +1038,7 @@
         <v>0.3200757575757576</v>
       </c>
       <c r="B84">
-        <v>-375.9945882173522</v>
+        <v>-247.4245662183944</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1046,7 +1046,7 @@
         <v>0.3299242424242425</v>
       </c>
       <c r="B85">
-        <v>-375.9945879490206</v>
+        <v>-247.4245659500628</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1054,7 +1054,7 @@
         <v>0.3397727272727273</v>
       </c>
       <c r="B86">
-        <v>-375.9945876806889</v>
+        <v>-247.4245656817311</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1062,7 +1062,7 @@
         <v>0.3496212121212121</v>
       </c>
       <c r="B87">
-        <v>-375.9945874123572</v>
+        <v>-247.4245654133994</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1070,7 +1070,7 @@
         <v>0.359469696969697</v>
       </c>
       <c r="B88">
-        <v>-375.9945871440256</v>
+        <v>-247.4245651450677</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1078,7 +1078,7 @@
         <v>0.3693181818181819</v>
       </c>
       <c r="B89">
-        <v>-375.9945868756938</v>
+        <v>-247.4245648767361</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1086,7 +1086,7 @@
         <v>0.3791666666666667</v>
       </c>
       <c r="B90">
-        <v>-375.9945866073622</v>
+        <v>-247.4245646084044</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1094,7 +1094,7 @@
         <v>0.3890151515151515</v>
       </c>
       <c r="B91">
-        <v>-375.9945863390305</v>
+        <v>-247.4245643400727</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1102,7 +1102,7 @@
         <v>0.3988636363636364</v>
       </c>
       <c r="B92">
-        <v>-375.9945860706989</v>
+        <v>-247.424564071741</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1110,7 +1110,7 @@
         <v>0.4087121212121213</v>
       </c>
       <c r="B93">
-        <v>-375.9945858023672</v>
+        <v>-247.4245638034094</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1118,7 +1118,7 @@
         <v>0.4185606060606061</v>
       </c>
       <c r="B94">
-        <v>-375.9945855340355</v>
+        <v>-247.4245635350777</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1126,7 +1126,7 @@
         <v>0.428409090909091</v>
       </c>
       <c r="B95">
-        <v>-375.9945852657039</v>
+        <v>-247.424563266746</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1134,7 +1134,7 @@
         <v>0.4382575757575758</v>
       </c>
       <c r="B96">
-        <v>-375.9945849973722</v>
+        <v>-247.4245629984144</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1142,7 +1142,7 @@
         <v>0.4481060606060606</v>
       </c>
       <c r="B97">
-        <v>-375.9945847290405</v>
+        <v>-247.4245627300827</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1150,7 +1150,7 @@
         <v>0.4579545454545455</v>
       </c>
       <c r="B98">
-        <v>-375.9945844607088</v>
+        <v>-247.424562461751</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1158,7 +1158,7 @@
         <v>0.4678030303030304</v>
       </c>
       <c r="B99">
-        <v>-375.9945841923771</v>
+        <v>-247.4245621934193</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1166,7 +1166,7 @@
         <v>0.4776515151515152</v>
       </c>
       <c r="B100">
-        <v>-375.9945839240454</v>
+        <v>-247.4245619250877</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1174,7 +1174,7 @@
         <v>0.4875</v>
       </c>
       <c r="B101">
-        <v>-375.9945836557138</v>
+        <v>-247.424561656756</v>
       </c>
     </row>
   </sheetData>

</xml_diff>